<commit_message>
Added few user stories.
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7938966-C893-4923-A742-8C0D4C1C2D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C38AF2-EC81-4B69-80E8-B27145432A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Διεργασία" sheetId="3" r:id="rId1"/>
     <sheet name="Product backlog Pithia" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
@@ -227,6 +227,24 @@
   </si>
   <si>
     <t>Πατώντας "Logout" εξέρχομαι από την εφαρμογή και ενημερώνεται ο λογαριασμός μου</t>
+  </si>
+  <si>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>Ως καθηγητης,θελω να εχω δυνατοτητα να βαζω βαθμολογια στους μαθητες που παρακολουθουν το μαθημα/μαθηματα που διδασκω.</t>
+  </si>
+  <si>
+    <t>Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" το οποιο θα οδηγει τον καθηγητη στη φορμα δηλωσης βαθμολογιας φοιτητων.</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>Ως διαχειριστης,θελω να εχω δυνατοτητα να προσθετω και να αφαιρω καθηγητη/-ες απο το συστημα.</t>
+  </si>
+  <si>
+    <t>Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Προσθηκη/Αφαιρεση Καθηγητη" το οποιο θα τον οδηγει στο περιβαλλον διαχειρισης καθηγητων.</t>
   </si>
 </sst>
 </file>
@@ -947,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1044,16 +1062,28 @@
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="39.950000000000003" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="89.45" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>

</xml_diff>